<commit_message>
handling exceptions when importing data from spread sheets
</commit_message>
<xml_diff>
--- a/Test_Paul.xlsx
+++ b/Test_Paul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speard\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F306E-280A-4ED8-B538-458C12219CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0391AD-22C2-4DAF-9FB8-55315BAC5DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>1/2" Shackle</t>
   </si>
@@ -74,9 +74,6 @@
     <t>off btm (m)</t>
   </si>
   <si>
-    <t>m Design Depth</t>
-  </si>
-  <si>
     <t>AR861 B2S</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
   </si>
   <si>
     <t>AF44↑ w WH150+SBE37 ODO</t>
-  </si>
-  <si>
-    <t>Chat3-4</t>
-  </si>
-  <si>
-    <t>July 2022</t>
   </si>
 </sst>
 </file>
@@ -427,10 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1088,326 +1078,309 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.61328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.69140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.69140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.15234375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.84375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.15234375" style="1"/>
+    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>160</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="5" customFormat="1" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="24">
         <f>362+86+4</f>
         <v>452</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C4" s="24">
         <f>-341+55+3</f>
         <v>-283</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D4" s="24">
         <v>2.13</v>
       </c>
-      <c r="E7" s="26">
-        <f>SUM(D7:D17)-0.3</f>
+      <c r="E4" s="25">
+        <f>SUM(D4:D14)-0.3</f>
         <v>10.02</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="26">
-        <f>$A$2-E7</f>
-        <v>149.97999999999999</v>
-      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="25" t="e">
+        <f>#REF!-E4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H4" s="54"/>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="21">
+        <v>0.37</v>
+      </c>
+      <c r="C5" s="19">
+        <f>(7.84-1)/7.84*B5</f>
+        <v>0.3228061224489796</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0.37</v>
+      </c>
+      <c r="C6" s="19">
+        <f>(7.84-1)/7.84*B6</f>
+        <v>0.3228061224489796</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="52"/>
+    </row>
+    <row r="7" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="21">
+        <v>1.23</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1.07</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="21">
         <v>0.37</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <f>(7.84-1)/7.84*B8</f>
         <v>0.3228061224489796</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>0.05</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="53"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="22">
-        <v>0.37</v>
-      </c>
-      <c r="C9" s="20">
-        <f>(7.84-1)/7.84*B9</f>
-        <v>0.3228061224489796</v>
-      </c>
-      <c r="D9" s="20">
-        <v>0.05</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="53"/>
-    </row>
-    <row r="10" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="22">
-        <v>1.23</v>
-      </c>
-      <c r="C10" s="20">
-        <v>1.07</v>
-      </c>
-      <c r="D10" s="20">
-        <v>0.15</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="56"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="22">
-        <v>0.37</v>
-      </c>
-      <c r="C11" s="20">
-        <f>(7.84-1)/7.84*B11</f>
-        <v>0.3228061224489796</v>
-      </c>
-      <c r="D11" s="20">
-        <v>0.05</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="53"/>
-    </row>
-    <row r="12" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="20">
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="52"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="19">
         <f>1.68/2.2</f>
         <v>0.76363636363636356</v>
       </c>
-      <c r="C12" s="20">
-        <f>(7.84-1)/7.84*B12</f>
+      <c r="C9" s="19">
+        <f>(7.84-1)/7.84*B9</f>
         <v>0.66623376623376618</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D9" s="19">
         <v>0.06</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="57"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="25">
+      <c r="E9" s="19"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="56"/>
+    </row>
+    <row r="10" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="24">
         <v>30</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C10" s="24">
         <v>22</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D10" s="24">
         <v>0.83</v>
       </c>
-      <c r="E13" s="25">
-        <f>SUM(D13:D17)</f>
+      <c r="E10" s="24">
+        <f>SUM(D10:D14)</f>
         <v>7.83</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="52"/>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C11" s="19">
+        <f>(7.84-1)/7.84*B11</f>
+        <v>2.0066326530612244</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="53"/>
+    </row>
+    <row r="12" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="22">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C14" s="20">
-        <f>(7.84-1)/7.84*B14</f>
-        <v>2.0066326530612244</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="54"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="35">
-        <f>0.285*D15</f>
+      <c r="B12" s="34">
+        <f>0.285*D12</f>
         <v>1.4249999999999998</v>
       </c>
-      <c r="C15" s="35">
-        <f>(0.91-1.027)/0.91*B15</f>
+      <c r="C12" s="34">
+        <f>(0.91-1.027)/0.91*B12</f>
         <v>-0.18321428571428552</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D12" s="29">
         <v>5</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="53"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="52"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B13" s="21">
         <v>1.8</v>
       </c>
-      <c r="C16" s="20">
-        <f>(7.84-1)/7.84*B16</f>
+      <c r="C13" s="19">
+        <f>(7.84-1)/7.84*B13</f>
         <v>1.5704081632653062</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="53"/>
-    </row>
-    <row r="17" spans="1:8" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="45" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="52"/>
+    </row>
+    <row r="14" spans="1:10" s="42" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B14" s="45">
         <f>85/2.2</f>
         <v>38.636363636363633</v>
       </c>
-      <c r="C17" s="46">
-        <f>(7.84-1)/7.84*B17</f>
+      <c r="C14" s="45">
+        <f>(7.84-1)/7.84*B14</f>
         <v>33.708256029684598</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D14" s="45">
         <v>2</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="53"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="50">
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="52"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H18" s="53"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="51"/>
-      <c r="C19" s="52"/>
+      <c r="H15" s="52"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1425,9 +1398,9 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1435,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>360</v>
       </c>
@@ -1443,7 +1416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>720</v>
       </c>
@@ -1451,7 +1424,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>3*360</f>
         <v>1080</v>
@@ -1475,7 +1448,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
got while loop working instead of for
</commit_message>
<xml_diff>
--- a/Test_Paul.xlsx
+++ b/Test_Paul.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0391AD-22C2-4DAF-9FB8-55315BAC5DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0D37EA-2A40-4871-89C3-4040021FF03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13068" yWindow="-2880" windowWidth="13176" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>1/2" Shackle</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Inst. Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estimated Amsteel II+ stretch   </t>
   </si>
   <si>
     <t>AF44↑ w WH150+SBE37 ODO</t>
@@ -418,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -497,8 +494,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1081,7 +1076,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1148,7 @@
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="24">
         <f>362+86+4</f>
@@ -1175,7 +1170,7 @@
         <f>#REF!-E4</f>
         <v>#REF!</v>
       </c>
-      <c r="H4" s="54"/>
+      <c r="H4" s="52"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -1194,7 +1189,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="22"/>
       <c r="G5" s="28"/>
-      <c r="H5" s="52"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -1213,7 +1208,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="22"/>
       <c r="G6" s="28"/>
-      <c r="H6" s="52"/>
+      <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
@@ -1231,7 +1226,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="22"/>
       <c r="G7" s="28"/>
-      <c r="H7" s="55"/>
+      <c r="H7" s="53"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
     </row>
@@ -1252,7 +1247,7 @@
       <c r="E8" s="36"/>
       <c r="F8" s="37"/>
       <c r="G8" s="38"/>
-      <c r="H8" s="52"/>
+      <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
@@ -1272,7 +1267,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="22"/>
       <c r="G9" s="40"/>
-      <c r="H9" s="56"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -1293,7 +1288,7 @@
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="52"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
@@ -1310,7 +1305,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="22"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="53"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
@@ -1330,7 +1325,7 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="30"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="50"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
@@ -1347,7 +1342,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="22"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="50"/>
     </row>
     <row r="14" spans="1:10" s="42" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44" t="s">
@@ -1367,20 +1362,19 @@
       <c r="E14" s="45"/>
       <c r="F14" s="46"/>
       <c r="G14" s="47"/>
-      <c r="H14" s="52"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="49">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H15" s="52"/>
+      <c r="A15" s="50"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Exception: an element does not exist in the database fixed for floats... prompts user to enter the element
</commit_message>
<xml_diff>
--- a/Test_Paul.xlsx
+++ b/Test_Paul.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0D37EA-2A40-4871-89C3-4040021FF03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13870BAE-FCBE-463D-BF3D-1F488D758420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13068" yWindow="-2880" windowWidth="13176" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1076,7 +1076,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>